<commit_message>
verificacion TAS y Sintactico
</commit_message>
<xml_diff>
--- a/TAS - SINTAXIS.xlsx
+++ b/TAS - SINTAXIS.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\sintaxis_proyecto_final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB1B7A4-EFE6-4239-B049-4A69AD3861AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="128">
   <si>
     <t>#</t>
   </si>
@@ -392,40 +401,44 @@
   </si>
   <si>
     <t>"/"&lt;EA3&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Escritura&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -436,7 +449,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -464,7 +477,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -478,51 +497,48 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf quotePrefix="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -712,23 +728,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AL40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="38" width="42.0"/>
+    <col min="1" max="20" width="42" customWidth="1"/>
+    <col min="21" max="21" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="38" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -842,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -878,7 +901,7 @@
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
-      <c r="AH2" s="5" t="s">
+      <c r="AH2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AI2" s="4"/>
@@ -886,7 +909,7 @@
       <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -919,7 +942,7 @@
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
       <c r="AD3" s="4"/>
-      <c r="AE3" s="5" t="s">
+      <c r="AE3" s="4" t="s">
         <v>40</v>
       </c>
       <c r="AF3" s="4"/>
@@ -930,7 +953,7 @@
       <c r="AK3" s="4"/>
       <c r="AL3" s="4"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
@@ -953,28 +976,28 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="4" t="s">
         <v>42</v>
       </c>
       <c r="V4" s="4"/>
-      <c r="W4" s="6" t="s">
+      <c r="W4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
-      <c r="Z4" s="6" t="s">
+      <c r="Z4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
-      <c r="AE4" s="6" t="s">
+      <c r="AE4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
-      <c r="AH4" s="6" t="s">
+      <c r="AH4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="AI4" s="4"/>
@@ -982,7 +1005,7 @@
       <c r="AK4" s="4"/>
       <c r="AL4" s="4"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -1018,51 +1041,51 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="5" t="s">
+      <c r="AH5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AI5" s="5" t="s">
+      <c r="AI5" s="4" t="s">
         <v>45</v>
       </c>
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>48</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="7" t="s">
+      <c r="Q6" s="6" t="s">
         <v>49</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="U6" s="4"/>
-      <c r="V6" s="6" t="s">
+      <c r="V6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="W6" s="4"/>
@@ -1076,7 +1099,7 @@
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
-      <c r="AH6" s="5" t="s">
+      <c r="AH6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="AI6" s="4"/>
@@ -1084,7 +1107,7 @@
       <c r="AK6" s="4"/>
       <c r="AL6" s="4"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1099,7 +1122,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N7" s="4"/>
@@ -1128,7 +1151,7 @@
       <c r="AK7" s="4"/>
       <c r="AL7" s="4"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
@@ -1143,7 +1166,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="5" t="s">
         <v>53</v>
       </c>
       <c r="N8" s="4"/>
@@ -1162,15 +1185,15 @@
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
-      <c r="AD8" s="6" t="s">
+      <c r="AD8" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AE8" s="4"/>
-      <c r="AF8" s="6" t="s">
+      <c r="AF8" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AG8" s="4"/>
-      <c r="AH8" s="5" t="s">
+      <c r="AH8" s="4" t="s">
         <v>53</v>
       </c>
       <c r="AI8" s="4"/>
@@ -1178,7 +1201,7 @@
       <c r="AK8" s="4"/>
       <c r="AL8" s="4"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -1193,7 +1216,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="4" t="s">
         <v>48</v>
       </c>
       <c r="N9" s="4"/>
@@ -1216,7 +1239,7 @@
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
-      <c r="AH9" s="5" t="s">
+      <c r="AH9" s="4" t="s">
         <v>55</v>
       </c>
       <c r="AI9" s="4"/>
@@ -1224,7 +1247,7 @@
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>56</v>
       </c>
@@ -1247,7 +1270,7 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
-      <c r="U10" s="5" t="s">
+      <c r="U10" s="4" t="s">
         <v>57</v>
       </c>
       <c r="V10" s="4"/>
@@ -1268,7 +1291,7 @@
       <c r="AK10" s="4"/>
       <c r="AL10" s="4"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
@@ -1300,15 +1323,15 @@
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
-      <c r="AD11" s="5" t="s">
+      <c r="AD11" s="4" t="s">
         <v>59</v>
       </c>
       <c r="AE11" s="4"/>
-      <c r="AF11" s="5" t="s">
+      <c r="AF11" s="4" t="s">
         <v>60</v>
       </c>
       <c r="AG11" s="4"/>
-      <c r="AH11" s="6" t="s">
+      <c r="AH11" s="5" t="s">
         <v>60</v>
       </c>
       <c r="AI11" s="4"/>
@@ -1316,19 +1339,19 @@
       <c r="AK11" s="4"/>
       <c r="AL11" s="4"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>63</v>
       </c>
       <c r="I12" s="4"/>
@@ -1342,11 +1365,11 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="8" t="s">
+      <c r="T12" s="7" t="s">
         <v>64</v>
       </c>
       <c r="U12" s="4"/>
-      <c r="V12" s="5" t="s">
+      <c r="V12" s="4" t="s">
         <v>65</v>
       </c>
       <c r="W12" s="4"/>
@@ -1360,7 +1383,7 @@
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
-      <c r="AH12" s="5" t="s">
+      <c r="AH12" s="4" t="s">
         <v>66</v>
       </c>
       <c r="AI12" s="4"/>
@@ -1368,7 +1391,7 @@
       <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
@@ -1383,7 +1406,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="5" t="s">
+      <c r="M13" s="4" t="s">
         <v>54</v>
       </c>
       <c r="N13" s="4"/>
@@ -1404,11 +1427,11 @@
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
-      <c r="AF13" s="5" t="s">
+      <c r="AF13" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AG13" s="4"/>
-      <c r="AH13" s="6" t="s">
+      <c r="AH13" s="5" t="s">
         <v>54</v>
       </c>
       <c r="AI13" s="4"/>
@@ -1416,7 +1439,7 @@
       <c r="AK13" s="4"/>
       <c r="AL13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>68</v>
       </c>
@@ -1431,7 +1454,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>69</v>
       </c>
       <c r="N14" s="4"/>
@@ -1460,7 +1483,7 @@
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>70</v>
       </c>
@@ -1483,70 +1506,70 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
-      <c r="U15" s="5" t="s">
+      <c r="U15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="V15" s="4"/>
-      <c r="W15" s="5" t="s">
+      <c r="W15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
-      <c r="Z15" s="5" t="s">
+      <c r="Z15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
-      <c r="AE15" s="5" t="s">
+      <c r="AE15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="AF15" s="4"/>
       <c r="AG15" s="4"/>
-      <c r="AH15" s="5" t="s">
+      <c r="AH15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="AI15" s="4"/>
-      <c r="AJ15" s="5" t="s">
+      <c r="AJ15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="AK15" s="4"/>
       <c r="AL15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="G16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="5" t="s">
+      <c r="R16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="S16" s="4"/>
@@ -1555,11 +1578,11 @@
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
-      <c r="Y16" s="5" t="s">
+      <c r="Y16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="Z16" s="4"/>
-      <c r="AA16" s="5" t="s">
+      <c r="AA16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="AB16" s="4"/>
@@ -1574,7 +1597,7 @@
       <c r="AK16" s="4"/>
       <c r="AL16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>74</v>
       </c>
@@ -1609,7 +1632,7 @@
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
-      <c r="AG17" s="5" t="s">
+      <c r="AG17" s="4" t="s">
         <v>75</v>
       </c>
       <c r="AH17" s="4"/>
@@ -1618,7 +1641,7 @@
       <c r="AK17" s="4"/>
       <c r="AL17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>76</v>
       </c>
@@ -1633,7 +1656,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="4" t="s">
         <v>77</v>
       </c>
       <c r="N18" s="4"/>
@@ -1652,15 +1675,15 @@
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
-      <c r="AD18" s="6" t="s">
+      <c r="AD18" s="5" t="s">
         <v>77</v>
       </c>
       <c r="AE18" s="4"/>
-      <c r="AF18" s="6" t="s">
+      <c r="AF18" s="5" t="s">
         <v>77</v>
       </c>
       <c r="AG18" s="4"/>
-      <c r="AH18" s="6" t="s">
+      <c r="AH18" s="5" t="s">
         <v>77</v>
       </c>
       <c r="AI18" s="4"/>
@@ -1668,7 +1691,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>78</v>
       </c>
@@ -1693,7 +1716,7 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
-      <c r="W19" s="5" t="s">
+      <c r="W19" s="4" t="s">
         <v>79</v>
       </c>
       <c r="X19" s="4"/>
@@ -1712,9 +1735,9 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1735,38 +1758,30 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
-      <c r="U20" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-      <c r="W20" s="5" t="s">
-        <v>82</v>
-      </c>
+      <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
-      <c r="Z20" s="5" t="s">
-        <v>83</v>
+      <c r="Z20" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
       <c r="AD20" s="4"/>
-      <c r="AE20" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
-      <c r="AH20" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="AH20" s="4"/>
       <c r="AI20" s="4"/>
       <c r="AJ20" s="4"/>
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1786,55 +1801,61 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="U21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
+      <c r="W21" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
+      <c r="Z21" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
-      <c r="AE21" s="4"/>
+      <c r="AE21" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
-      <c r="AH21" s="4"/>
+      <c r="AH21" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="AI21" s="4"/>
       <c r="AJ21" s="4"/>
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
+      <c r="T22" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
@@ -1854,25 +1875,27 @@
       <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="N23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -1886,9 +1909,7 @@
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
-      <c r="AB23" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
@@ -1900,74 +1921,66 @@
       <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
-      <c r="T24" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="T24" s="4"/>
       <c r="U24" s="4"/>
-      <c r="V24" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
-      <c r="Z24" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
-      <c r="AB24" s="4"/>
+      <c r="AB24" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="AC24" s="4"/>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
       <c r="AG24" s="4"/>
-      <c r="AH24" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="AH24" s="4"/>
       <c r="AI24" s="4"/>
       <c r="AJ24" s="4"/>
       <c r="AK24" s="4"/>
       <c r="AL24" s="4"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="6" t="s">
-        <v>95</v>
+      <c r="C25" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="6" t="s">
-        <v>95</v>
+      <c r="H25" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1980,17 +1993,16 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
-      <c r="T25" s="6" t="s">
-        <v>95</v>
+      <c r="T25" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="U25" s="4"/>
-      <c r="V25" s="6" t="s">
-        <v>95</v>
+      <c r="V25" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
@@ -1999,27 +2011,27 @@
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
       <c r="AH25" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AI25" s="4"/>
       <c r="AJ25" s="4"/>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:38" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="6" t="s">
-        <v>97</v>
+      <c r="H26" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -2032,12 +2044,12 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
-      <c r="T26" s="6" t="s">
-        <v>97</v>
+      <c r="T26" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="U26" s="4"/>
-      <c r="V26" s="6" t="s">
-        <v>97</v>
+      <c r="V26" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
@@ -2050,45 +2062,47 @@
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
-      <c r="AH26" s="6" t="s">
-        <v>97</v>
+      <c r="AH26" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="AI26" s="4"/>
       <c r="AJ26" s="4"/>
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="H27" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-      <c r="P27" s="5" t="s">
-        <v>101</v>
-      </c>
+      <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
+      <c r="T27" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
+      <c r="V27" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
@@ -2100,66 +2114,50 @@
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
-      <c r="AH27" s="4"/>
+      <c r="AH27" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="AI27" s="4"/>
       <c r="AJ27" s="4"/>
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="P28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="Q28" s="4"/>
-      <c r="R28" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="R28" s="4"/>
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
-      <c r="Y28" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
-      <c r="AA28" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA28" s="4"/>
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
       <c r="AD28" s="4"/>
@@ -2172,46 +2170,62 @@
       <c r="AK28" s="4"/>
       <c r="AL28" s="4"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="J29" s="4"/>
-      <c r="K29" s="5" t="s">
+      <c r="K29" s="4" t="s">
         <v>45</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
+      <c r="N29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
+      <c r="R29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
+      <c r="Y29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
+      <c r="AA29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AB29" s="4"/>
-      <c r="AC29" s="5" t="s">
-        <v>105</v>
-      </c>
+      <c r="AC29" s="4"/>
       <c r="AD29" s="4"/>
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
@@ -2219,96 +2233,98 @@
       <c r="AH29" s="4"/>
       <c r="AI29" s="4"/>
       <c r="AJ29" s="4"/>
-      <c r="AK29" s="5" t="s">
-        <v>106</v>
-      </c>
+      <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="5"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="G30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="K30" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L30" s="4"/>
-      <c r="M30" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-      <c r="Q30" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
-      <c r="T30" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="T30" s="4"/>
       <c r="U30" s="4"/>
-      <c r="V30" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="V30" s="4"/>
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
-      <c r="AC30" s="4"/>
+      <c r="AC30" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
       <c r="AG30" s="4"/>
-      <c r="AH30" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="AH30" s="4"/>
       <c r="AI30" s="4"/>
       <c r="AJ30" s="4"/>
-      <c r="AK30" s="4"/>
+      <c r="AK30" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="AL30" s="4"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="C31" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="M31" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
+      <c r="Q31" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
+      <c r="T31" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
+      <c r="V31" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
       <c r="Y31" s="4"/>
@@ -2320,27 +2336,29 @@
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
-      <c r="AH31" s="4"/>
+      <c r="AH31" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="AI31" s="4"/>
       <c r="AJ31" s="4"/>
       <c r="AK31" s="4"/>
       <c r="AL31" s="4"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="5" t="s">
-        <v>112</v>
-      </c>
+      <c r="G32" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -2352,13 +2370,9 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
-      <c r="T32" s="5" t="s">
-        <v>112</v>
-      </c>
+      <c r="T32" s="4"/>
       <c r="U32" s="4"/>
-      <c r="V32" s="5" t="s">
-        <v>112</v>
-      </c>
+      <c r="V32" s="4"/>
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
       <c r="Y32" s="4"/>
@@ -2370,25 +2384,27 @@
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
       <c r="AG32" s="4"/>
-      <c r="AH32" s="5" t="s">
-        <v>112</v>
-      </c>
+      <c r="AH32" s="4"/>
       <c r="AI32" s="4"/>
       <c r="AJ32" s="4"/>
       <c r="AK32" s="4"/>
       <c r="AL32" s="4"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="H33" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -2399,61 +2415,47 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
-      <c r="S33" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="T33" s="4"/>
-      <c r="U33" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="V33" s="4"/>
-      <c r="W33" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="W33" s="4"/>
       <c r="X33" s="4"/>
       <c r="Y33" s="4"/>
-      <c r="Z33" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="Z33" s="4"/>
       <c r="AA33" s="4"/>
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
       <c r="AD33" s="4"/>
-      <c r="AE33" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
-      <c r="AH33" s="5" t="s">
-        <v>45</v>
+      <c r="AH33" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="AI33" s="4"/>
-      <c r="AJ33" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="AJ33" s="4"/>
       <c r="AK33" s="4"/>
       <c r="AL33" s="4"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2461,51 +2463,63 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
+      <c r="S34" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
+      <c r="U34" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="5" t="s">
-        <v>116</v>
-      </c>
+      <c r="W34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
+      <c r="Z34" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AA34" s="4"/>
       <c r="AB34" s="4"/>
-      <c r="AC34" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="AC34" s="4"/>
       <c r="AD34" s="4"/>
-      <c r="AE34" s="4"/>
+      <c r="AE34" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
-      <c r="AH34" s="4"/>
+      <c r="AH34" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AI34" s="4"/>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="AJ34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="K35" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L35" s="4"/>
-      <c r="M35" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
@@ -2516,12 +2530,16 @@
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
       <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
+      <c r="X35" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="Y35" s="4"/>
       <c r="Z35" s="4"/>
       <c r="AA35" s="4"/>
       <c r="AB35" s="4"/>
-      <c r="AC35" s="4"/>
+      <c r="AC35" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AD35" s="4"/>
       <c r="AE35" s="4"/>
       <c r="AF35" s="4"/>
@@ -2529,30 +2547,30 @@
       <c r="AH35" s="4"/>
       <c r="AI35" s="4"/>
       <c r="AJ35" s="4"/>
-      <c r="AK35" s="4"/>
+      <c r="AK35" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AL35" s="4"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="M36" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
@@ -2578,62 +2596,40 @@
       <c r="AK36" s="4"/>
       <c r="AL36" s="4"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O37" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="R37" s="4"/>
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
-      <c r="Y37" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
-      <c r="AA37" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA37" s="4"/>
       <c r="AB37" s="4"/>
       <c r="AC37" s="4"/>
       <c r="AD37" s="4"/>
@@ -2646,123 +2642,191 @@
       <c r="AK37" s="4"/>
       <c r="AL37" s="4"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B38" s="4"/>
-      <c r="C38" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="K38" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
+      <c r="M38" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
+      <c r="R38" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S38" s="4"/>
-      <c r="T38" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="T38" s="4"/>
       <c r="U38" s="4"/>
-      <c r="V38" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="V38" s="4"/>
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
+      <c r="Y38" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="Z38" s="4"/>
-      <c r="AA38" s="4"/>
+      <c r="AA38" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AB38" s="4"/>
       <c r="AC38" s="4"/>
       <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
       <c r="AF38" s="4"/>
       <c r="AG38" s="4"/>
-      <c r="AH38" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="AH38" s="4"/>
       <c r="AI38" s="4"/>
       <c r="AJ38" s="4"/>
       <c r="AK38" s="4"/>
       <c r="AL38" s="4"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="C39" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I39" s="4"/>
       <c r="J39" s="4"/>
-      <c r="K39" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
-      <c r="N39" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
-      <c r="R39" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="R39" s="4"/>
       <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
+      <c r="T39" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
+      <c r="V39" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
-      <c r="Y39" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
-      <c r="AA39" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA39" s="4"/>
       <c r="AB39" s="4"/>
       <c r="AC39" s="4"/>
       <c r="AD39" s="4"/>
       <c r="AE39" s="4"/>
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
-      <c r="AH39" s="4"/>
+      <c r="AH39" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="AI39" s="4"/>
       <c r="AJ39" s="4"/>
       <c r="AK39" s="4"/>
       <c r="AL39" s="4"/>
     </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB40" s="4"/>
+      <c r="AC40" s="4"/>
+      <c r="AD40" s="4"/>
+      <c r="AE40" s="4"/>
+      <c r="AF40" s="4"/>
+      <c r="AG40" s="4"/>
+      <c r="AH40" s="4"/>
+      <c r="AI40" s="4"/>
+      <c r="AJ40" s="4"/>
+      <c r="AK40" s="4"/>
+      <c r="AL40" s="4"/>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
programas a entregar v1
</commit_message>
<xml_diff>
--- a/TAS - SINTAXIS.xlsx
+++ b/TAS - SINTAXIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\sintaxis_proyecto_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB1B7A4-EFE6-4239-B049-4A69AD3861AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59424D58-8224-4542-96DA-35F40784DF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -751,7 +751,7 @@
     <col min="22" max="38" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -865,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -909,7 +909,7 @@
       <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -953,7 +953,7 @@
       <c r="AK3" s="4"/>
       <c r="AL3" s="4"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
@@ -1005,7 +1005,7 @@
       <c r="AK4" s="4"/>
       <c r="AL4" s="4"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -1051,7 +1051,7 @@
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1107,7 +1107,7 @@
       <c r="AK6" s="4"/>
       <c r="AL6" s="4"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1151,7 +1151,7 @@
       <c r="AK7" s="4"/>
       <c r="AL7" s="4"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
@@ -1201,7 +1201,7 @@
       <c r="AK8" s="4"/>
       <c r="AL8" s="4"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -1247,7 +1247,7 @@
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>56</v>
       </c>
@@ -1291,7 +1291,7 @@
       <c r="AK10" s="4"/>
       <c r="AL10" s="4"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
@@ -1339,7 +1339,7 @@
       <c r="AK11" s="4"/>
       <c r="AL11" s="4"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>61</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
@@ -1439,7 +1439,7 @@
       <c r="AK13" s="4"/>
       <c r="AL13" s="4"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>68</v>
       </c>
@@ -1483,7 +1483,7 @@
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>70</v>
       </c>
@@ -1537,7 +1537,7 @@
       <c r="AK15" s="4"/>
       <c r="AL15" s="4"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>71</v>
       </c>
@@ -1597,7 +1597,7 @@
       <c r="AK16" s="4"/>
       <c r="AL16" s="4"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>74</v>
       </c>
@@ -1641,7 +1641,7 @@
       <c r="AK17" s="4"/>
       <c r="AL17" s="4"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>76</v>
       </c>
@@ -1691,7 +1691,7 @@
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>78</v>
       </c>
@@ -1779,7 +1779,7 @@
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>80</v>
       </c>
@@ -1831,7 +1831,7 @@
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
@@ -1875,7 +1875,7 @@
       <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>87</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>89</v>
       </c>
@@ -2070,7 +2070,7 @@
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>96</v>
       </c>
@@ -2122,7 +2122,7 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>98</v>
       </c>
@@ -2170,7 +2170,7 @@
       <c r="AK28" s="4"/>
       <c r="AL28" s="4"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>102</v>
       </c>
@@ -2236,7 +2236,7 @@
       <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>104</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="AL30" s="4"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>107</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="AK31" s="4"/>
       <c r="AL31" s="4"/>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>109</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="AK32" s="4"/>
       <c r="AL32" s="4"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>111</v>
       </c>
@@ -2442,7 +2442,7 @@
       <c r="AK33" s="4"/>
       <c r="AL33" s="4"/>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>113</v>
       </c>
@@ -2498,7 +2498,7 @@
       <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>115</v>
       </c>
@@ -2552,7 +2552,7 @@
       </c>
       <c r="AL35" s="4"/>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -2596,7 +2596,7 @@
       <c r="AK36" s="4"/>
       <c r="AL36" s="4"/>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>118</v>
       </c>
@@ -2642,7 +2642,7 @@
       <c r="AK37" s="4"/>
       <c r="AL37" s="4"/>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>120</v>
       </c>
@@ -2710,7 +2710,7 @@
       <c r="AK38" s="4"/>
       <c r="AL38" s="4"/>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>122</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="AK39" s="4"/>
       <c r="AL39" s="4"/>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
pruebas en los programas
</commit_message>
<xml_diff>
--- a/TAS - SINTAXIS.xlsx
+++ b/TAS - SINTAXIS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\sintaxis_proyecto_final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FedeF\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59424D58-8224-4542-96DA-35F40784DF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{30BB5ED7-1D09-4D64-88FB-0C7F5B59949A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="120">
   <si>
     <t>#</t>
   </si>
@@ -178,15 +178,6 @@
     <t>'[''&lt;Columnas&gt;'']''&lt;FacFilas&gt;</t>
   </si>
   <si>
-    <t>&lt;EM1&gt;</t>
-  </si>
-  <si>
-    <t>&lt;EM2&gt;&lt;M2&gt;</t>
-  </si>
-  <si>
-    <t>&lt;EMM&gt;</t>
-  </si>
-  <si>
     <t>"id"</t>
   </si>
   <si>
@@ -196,15 +187,6 @@
     <t>"if"&lt;Cond&gt;"then""{"&lt;Cuerpo&gt;"}"&lt;FacCondicional&gt;</t>
   </si>
   <si>
-    <t>&lt;EM2&gt;</t>
-  </si>
-  <si>
-    <t>Tr"("&lt;EM&gt;")"</t>
-  </si>
-  <si>
-    <t>&lt;EM3&gt;</t>
-  </si>
-  <si>
     <t>&lt;EA4&gt;</t>
   </si>
   <si>
@@ -223,9 +205,6 @@
     <t>"id"&lt;E4&gt;</t>
   </si>
   <si>
-    <t>"ProdEscMat""("&lt;EA1&gt;","&lt;EM&gt;")"</t>
-  </si>
-  <si>
     <t>&lt;MatrizReal&gt;</t>
   </si>
   <si>
@@ -253,9 +232,6 @@
     <t>&lt;EM&gt;</t>
   </si>
   <si>
-    <t>&lt;EM1&gt;&lt;M1&gt;</t>
-  </si>
-  <si>
     <t>&lt;Lectura&gt;</t>
   </si>
   <si>
@@ -334,15 +310,6 @@
     <t xml:space="preserve">"^" &lt;EA4&gt; </t>
   </si>
   <si>
-    <t>&lt;M1&gt;</t>
-  </si>
-  <si>
-    <t>"SumaMat" "(" &lt;EM&gt; "," &lt;EM&gt; ")"</t>
-  </si>
-  <si>
-    <t>"RestaMat" "(" &lt;EM&gt; "," &lt;EM&gt; ")"</t>
-  </si>
-  <si>
     <t>&lt;listaElementos&gt;</t>
   </si>
   <si>
@@ -367,12 +334,6 @@
     <t>"else""{"&lt;Cuerpo&gt;"}"</t>
   </si>
   <si>
-    <t>&lt;M2&gt;</t>
-  </si>
-  <si>
-    <t>"MultMat""("&lt;EM&gt;","&lt;EM&gt;")"</t>
-  </si>
-  <si>
     <t>"["&lt;Filas&gt;"]"</t>
   </si>
   <si>
@@ -404,6 +365,21 @@
   </si>
   <si>
     <t>&lt;Escritura&gt;</t>
+  </si>
+  <si>
+    <t>SumMat "(" &lt;EM&gt; "," &lt;EM&gt; )"</t>
+  </si>
+  <si>
+    <t>RestMat "(" &lt;EM&gt; "," &lt;EM&gt; )"</t>
+  </si>
+  <si>
+    <t>MultMat "(" &lt;EM&gt; "," &lt;EM&gt; )"</t>
+  </si>
+  <si>
+    <t>"Tr" "(" &lt;EM&gt; ")"</t>
+  </si>
+  <si>
+    <t>"ProdEscMat" ( &lt;EA1&gt; "," &lt;EM&gt; )</t>
   </si>
 </sst>
 </file>
@@ -738,20 +714,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AL40"/>
+  <dimension ref="A1:AL35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="20" width="42" customWidth="1"/>
-    <col min="21" max="21" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="52.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="38" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -865,7 +841,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -909,7 +885,7 @@
       <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
     </row>
-    <row r="3" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -953,7 +929,7 @@
       <c r="AK3" s="4"/>
       <c r="AL3" s="4"/>
     </row>
-    <row r="4" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
@@ -1005,7 +981,7 @@
       <c r="AK4" s="4"/>
       <c r="AL4" s="4"/>
     </row>
-    <row r="5" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -1051,7 +1027,7 @@
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
     </row>
-    <row r="6" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1107,7 +1083,7 @@
       <c r="AK6" s="4"/>
       <c r="AL6" s="4"/>
     </row>
-    <row r="7" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1151,9 +1127,9 @@
       <c r="AK7" s="4"/>
       <c r="AL7" s="4"/>
     </row>
-    <row r="8" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1166,9 +1142,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -1176,7 +1150,9 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
+      <c r="U8" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
@@ -1185,49 +1161,49 @@
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
-      <c r="AD8" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
-      <c r="AF8" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
-      <c r="AH8" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
       <c r="AK8" s="4"/>
       <c r="AL8" s="4"/>
     </row>
-    <row r="9" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
+      <c r="T9" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
+      <c r="V9" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -1240,16 +1216,16 @@
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
       <c r="AH9" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AI9" s="4"/>
       <c r="AJ9" s="4"/>
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
     </row>
-    <row r="10" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1262,7 +1238,9 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -1270,9 +1248,7 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
-      <c r="U10" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
@@ -1291,9 +1267,9 @@
       <c r="AK10" s="4"/>
       <c r="AL10" s="4"/>
     </row>
-    <row r="11" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1314,86 +1290,100 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
+      <c r="U11" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
+      <c r="W11" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
+      <c r="Z11" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
-      <c r="AD11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE11" s="4"/>
-      <c r="AF11" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF11" s="4"/>
       <c r="AG11" s="4"/>
-      <c r="AH11" s="5" t="s">
-        <v>60</v>
+      <c r="AH11" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="AI11" s="4"/>
-      <c r="AJ11" s="4"/>
+      <c r="AJ11" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AK11" s="4"/>
       <c r="AL11" s="4"/>
     </row>
-    <row r="12" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="H12" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="N12" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="R12" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S12" s="4"/>
-      <c r="T12" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="T12" s="4"/>
       <c r="U12" s="4"/>
-      <c r="V12" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
+      <c r="Y12" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
+      <c r="AA12" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
-      <c r="AH12" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
       <c r="AJ12" s="4"/>
       <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
     </row>
-    <row r="13" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1406,9 +1396,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -1427,21 +1415,19 @@
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
-      <c r="AF13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG13" s="4"/>
-      <c r="AH13" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH13" s="4"/>
       <c r="AI13" s="4"/>
       <c r="AJ13" s="4"/>
       <c r="AK13" s="4"/>
       <c r="AL13" s="4"/>
     </row>
-    <row r="14" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1455,7 +1441,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1467,23 +1453,35 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
+      <c r="X14" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
+      <c r="AC14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="AE14" s="4"/>
-      <c r="AF14" s="4"/>
+      <c r="AF14" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="AG14" s="4"/>
-      <c r="AH14" s="4"/>
+      <c r="AH14" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="AI14" s="4"/>
       <c r="AJ14" s="4"/>
-      <c r="AK14" s="4"/>
+      <c r="AK14" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="AL14" s="4"/>
     </row>
-    <row r="15" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>70</v>
       </c>
@@ -1506,85 +1504,59 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
-      <c r="U15" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
-      <c r="Z15" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
-      <c r="AE15" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
       <c r="AG15" s="4"/>
-      <c r="AH15" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="AH15" s="4"/>
       <c r="AI15" s="4"/>
-      <c r="AJ15" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="AJ15" s="4"/>
       <c r="AK15" s="4"/>
       <c r="AL15" s="4"/>
     </row>
-    <row r="16" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
-      <c r="Y16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
       <c r="AD16" s="4"/>
@@ -1597,9 +1569,9 @@
       <c r="AK16" s="4"/>
       <c r="AL16" s="4"/>
     </row>
-    <row r="17" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1620,30 +1592,38 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
+      <c r="U17" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
+      <c r="W17" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
+      <c r="Z17" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="AA17" s="4"/>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
       <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
+      <c r="AE17" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="AF17" s="4"/>
-      <c r="AG17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="AI17" s="4"/>
       <c r="AJ17" s="4"/>
       <c r="AK17" s="4"/>
       <c r="AL17" s="4"/>
     </row>
-    <row r="18" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1656,16 +1636,16 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
+      <c r="T18" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
@@ -1675,39 +1655,37 @@
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
-      <c r="AD18" s="5" t="s">
-        <v>77</v>
-      </c>
+      <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
-      <c r="AF18" s="5" t="s">
-        <v>77</v>
-      </c>
+      <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
-      <c r="AH18" s="5" t="s">
-        <v>77</v>
-      </c>
+      <c r="AH18" s="4"/>
       <c r="AI18" s="4"/>
       <c r="AJ18" s="4"/>
       <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
     </row>
-    <row r="19" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
@@ -1716,9 +1694,7 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
-      <c r="W19" s="4" t="s">
-        <v>79</v>
-      </c>
+      <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
@@ -1735,9 +1711,9 @@
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
     </row>
-    <row r="20" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1750,7 +1726,9 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
@@ -1763,11 +1741,11 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
-      <c r="Z20" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
+      <c r="AB20" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="AC20" s="4"/>
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
@@ -1779,17 +1757,21 @@
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
     </row>
-    <row r="21" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1801,47 +1783,46 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="T21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="U21" s="4"/>
+      <c r="V21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
-      <c r="AE21" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
-      <c r="AH21" s="4" t="s">
-        <v>85</v>
+      <c r="AH21" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="AI21" s="4"/>
       <c r="AJ21" s="4"/>
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
     </row>
-    <row r="22" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="C22" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="H22" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1853,11 +1834,13 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
-      <c r="T22" s="4" t="s">
-        <v>86</v>
+      <c r="T22" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
+      <c r="V22" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
@@ -1869,41 +1852,47 @@
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
-      <c r="AH22" s="4"/>
+      <c r="AH22" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="AI22" s="4"/>
       <c r="AJ22" s="4"/>
       <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
     </row>
-    <row r="23" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
+      <c r="T23" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
+      <c r="V23" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
@@ -1915,15 +1904,17 @@
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
-      <c r="AH23" s="4"/>
+      <c r="AH23" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="AI23" s="4"/>
       <c r="AJ23" s="4"/>
       <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
     </row>
-    <row r="24" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1935,13 +1926,17 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="L24" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="M24" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
+      <c r="P24" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
@@ -1953,9 +1948,7 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
-      <c r="AB24" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
@@ -1967,89 +1960,108 @@
       <c r="AK24" s="4"/>
       <c r="AL24" s="4"/>
     </row>
-    <row r="25" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="K25" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
+      <c r="N25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
+      <c r="R25" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S25" s="4"/>
-      <c r="T25" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="T25" s="4"/>
       <c r="U25" s="4"/>
-      <c r="V25" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="AA25" s="4"/>
+      <c r="Y25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
-      <c r="AH25" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="AH25" s="4"/>
       <c r="AI25" s="4"/>
       <c r="AJ25" s="4"/>
       <c r="AK25" s="4"/>
       <c r="AL25" s="4"/>
     </row>
-    <row r="26" spans="1:38" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="5" t="s">
-        <v>95</v>
+      <c r="C26" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="5" t="s">
-        <v>95</v>
+      <c r="H26" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="M26" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
+      <c r="Q26" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
-      <c r="T26" s="5" t="s">
-        <v>95</v>
+      <c r="T26" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="U26" s="4"/>
-      <c r="V26" s="5" t="s">
-        <v>95</v>
+      <c r="V26" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
@@ -2063,28 +2075,28 @@
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
       <c r="AH26" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AI26" s="4"/>
       <c r="AJ26" s="4"/>
       <c r="AK26" s="4"/>
       <c r="AL26" s="4"/>
     </row>
-    <row r="27" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="G27" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -2096,13 +2108,9 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
-      <c r="T27" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="T27" s="4"/>
       <c r="U27" s="4"/>
-      <c r="V27" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
@@ -2114,45 +2122,45 @@
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
-      <c r="AH27" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="AH27" s="4"/>
       <c r="AI27" s="4"/>
       <c r="AJ27" s="4"/>
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
     </row>
-    <row r="28" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="4" t="s">
-        <v>101</v>
-      </c>
+      <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
+      <c r="T28" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
+      <c r="V28" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
       <c r="Y28" s="4"/>
@@ -2164,100 +2172,88 @@
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
       <c r="AG28" s="4"/>
-      <c r="AH28" s="4"/>
+      <c r="AH28" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="AI28" s="4"/>
       <c r="AJ28" s="4"/>
       <c r="AK28" s="4"/>
       <c r="AL28" s="4"/>
     </row>
-    <row r="29" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
-      <c r="R29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="S29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
+      <c r="U29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
+      <c r="W29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="X29" s="4"/>
-      <c r="Y29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z29" s="4"/>
-      <c r="AA29" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
       <c r="AC29" s="4"/>
       <c r="AD29" s="4"/>
-      <c r="AE29" s="4"/>
+      <c r="AE29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
-      <c r="AH29" s="4"/>
+      <c r="AH29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AI29" s="4"/>
-      <c r="AJ29" s="4"/>
+      <c r="AJ29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AK29" s="4"/>
       <c r="AL29" s="4"/>
     </row>
-    <row r="30" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
@@ -2273,9 +2269,7 @@
       <c r="Z30" s="4"/>
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
-      <c r="AC30" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="AC30" s="4"/>
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
@@ -2283,48 +2277,38 @@
       <c r="AH30" s="4"/>
       <c r="AI30" s="4"/>
       <c r="AJ30" s="4"/>
-      <c r="AK30" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="AK30" s="4"/>
       <c r="AL30" s="4"/>
     </row>
-    <row r="31" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="G31" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="N31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
-      <c r="Q31" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
-      <c r="T31" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="T31" s="4"/>
       <c r="U31" s="4"/>
-      <c r="V31" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="V31" s="4"/>
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
       <c r="Y31" s="4"/>
@@ -2336,48 +2320,68 @@
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
-      <c r="AH31" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="AH31" s="4"/>
       <c r="AI31" s="4"/>
       <c r="AJ31" s="4"/>
       <c r="AK31" s="4"/>
       <c r="AL31" s="4"/>
     </row>
-    <row r="32" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="G32" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="K32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
+      <c r="M32" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
+      <c r="R32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
+      <c r="Y32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
+      <c r="AA32" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AB32" s="4"/>
       <c r="AC32" s="4"/>
       <c r="AD32" s="4"/>
@@ -2390,20 +2394,20 @@
       <c r="AK32" s="4"/>
       <c r="AL32" s="4"/>
     </row>
-    <row r="33" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -2417,11 +2421,11 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
       <c r="T33" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="U33" s="4"/>
       <c r="V33" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="W33" s="4"/>
       <c r="X33" s="4"/>
@@ -2435,397 +2439,78 @@
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
       <c r="AH33" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AI33" s="4"/>
       <c r="AJ33" s="4"/>
       <c r="AK33" s="4"/>
       <c r="AL33" s="4"/>
     </row>
-    <row r="34" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="K34" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
+      <c r="N34" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="R34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S34" s="4"/>
       <c r="T34" s="4"/>
-      <c r="U34" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="U34" s="4"/>
       <c r="V34" s="4"/>
-      <c r="W34" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="W34" s="4"/>
       <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA34" s="4"/>
+      <c r="Y34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="AB34" s="4"/>
       <c r="AC34" s="4"/>
       <c r="AD34" s="4"/>
-      <c r="AE34" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
-      <c r="AH34" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="AH34" s="4"/>
       <c r="AI34" s="4"/>
-      <c r="AJ34" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="AJ34" s="4"/>
       <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
     </row>
-    <row r="35" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-      <c r="AA35" s="4"/>
-      <c r="AB35" s="4"/>
-      <c r="AC35" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD35" s="4"/>
-      <c r="AE35" s="4"/>
-      <c r="AF35" s="4"/>
-      <c r="AG35" s="4"/>
-      <c r="AH35" s="4"/>
-      <c r="AI35" s="4"/>
-      <c r="AJ35" s="4"/>
-      <c r="AK35" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL35" s="4"/>
-    </row>
-    <row r="36" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
-      <c r="AA36" s="4"/>
-      <c r="AB36" s="4"/>
-      <c r="AC36" s="4"/>
-      <c r="AD36" s="4"/>
-      <c r="AE36" s="4"/>
-      <c r="AF36" s="4"/>
-      <c r="AG36" s="4"/>
-      <c r="AH36" s="4"/>
-      <c r="AI36" s="4"/>
-      <c r="AJ36" s="4"/>
-      <c r="AK36" s="4"/>
-      <c r="AL36" s="4"/>
-    </row>
-    <row r="37" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
-      <c r="AC37" s="4"/>
-      <c r="AD37" s="4"/>
-      <c r="AE37" s="4"/>
-      <c r="AF37" s="4"/>
-      <c r="AG37" s="4"/>
-      <c r="AH37" s="4"/>
-      <c r="AI37" s="4"/>
-      <c r="AJ37" s="4"/>
-      <c r="AK37" s="4"/>
-      <c r="AL37" s="4"/>
-    </row>
-    <row r="38" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-      <c r="X38" s="4"/>
-      <c r="Y38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z38" s="4"/>
-      <c r="AA38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB38" s="4"/>
-      <c r="AC38" s="4"/>
-      <c r="AD38" s="4"/>
-      <c r="AE38" s="4"/>
-      <c r="AF38" s="4"/>
-      <c r="AG38" s="4"/>
-      <c r="AH38" s="4"/>
-      <c r="AI38" s="4"/>
-      <c r="AJ38" s="4"/>
-      <c r="AK38" s="4"/>
-      <c r="AL38" s="4"/>
-    </row>
-    <row r="39" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="W39" s="4"/>
-      <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-      <c r="Z39" s="4"/>
-      <c r="AA39" s="4"/>
-      <c r="AB39" s="4"/>
-      <c r="AC39" s="4"/>
-      <c r="AD39" s="4"/>
-      <c r="AE39" s="4"/>
-      <c r="AF39" s="4"/>
-      <c r="AG39" s="4"/>
-      <c r="AH39" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AI39" s="4"/>
-      <c r="AJ39" s="4"/>
-      <c r="AK39" s="4"/>
-      <c r="AL39" s="4"/>
-    </row>
-    <row r="40" spans="1:38" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
-      <c r="W40" s="4"/>
-      <c r="X40" s="4"/>
-      <c r="Y40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z40" s="4"/>
-      <c r="AA40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB40" s="4"/>
-      <c r="AC40" s="4"/>
-      <c r="AD40" s="4"/>
-      <c r="AE40" s="4"/>
-      <c r="AF40" s="4"/>
-      <c r="AG40" s="4"/>
-      <c r="AH40" s="4"/>
-      <c r="AI40" s="4"/>
-      <c r="AJ40" s="4"/>
-      <c r="AK40" s="4"/>
-      <c r="AL40" s="4"/>
-    </row>
+    <row r="35" spans="1:38" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>